<commit_message>
Correction EN intake system
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/EN/ENA0200_to_ENA0400.xlsx
+++ b/CR - Cost Report/BOM/EN/ENA0200_to_ENA0400.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>System</t>
   </si>
@@ -221,9 +221,6 @@
     <t>EN_04009</t>
   </si>
   <si>
-    <t>EN_04010</t>
-  </si>
-  <si>
     <t>Inferior plate</t>
   </si>
   <si>
@@ -260,12 +257,6 @@
     <t>Convergent</t>
   </si>
   <si>
-    <t>Ring spacer</t>
-  </si>
-  <si>
-    <t>For the throttle sensor</t>
-  </si>
-  <si>
     <t>Frame mounting tube</t>
   </si>
   <si>
@@ -314,9 +305,6 @@
     <t>Link up the guillotine to the air intake</t>
   </si>
   <si>
-    <t>Joint gaskets</t>
-  </si>
-  <si>
     <t>Under the restrictor</t>
   </si>
   <si>
@@ -333,6 +321,9 @@
   </si>
   <si>
     <t>Mounting plate</t>
+  </si>
+  <si>
+    <t>Exhaust flange</t>
   </si>
 </sst>
 </file>
@@ -757,11 +748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="I1:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +767,7 @@
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -814,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -832,16 +823,8 @@
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3">
-        <f>LEN(C3)</f>
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <f>LEN(E3)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -859,16 +842,8 @@
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I32" si="0">LEN(C4)</f>
-        <v>18</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J32" si="1">LEN(E4)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -886,16 +861,8 @@
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -913,26 +880,18 @@
       <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -940,26 +899,18 @@
       <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -967,20 +918,12 @@
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>38</v>
@@ -994,26 +937,18 @@
       <c r="G9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F10" s="4">
         <v>4</v>
@@ -1021,16 +956,8 @@
       <c r="G10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1048,26 +975,18 @@
       <c r="G11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1075,16 +994,8 @@
       <c r="G12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1098,26 +1009,18 @@
       <c r="G13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1125,16 +1028,8 @@
       <c r="G14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -1144,7 +1039,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -1152,16 +1047,8 @@
       <c r="G15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -1171,7 +1058,7 @@
         <v>36</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1179,16 +1066,8 @@
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -1198,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -1206,26 +1085,18 @@
       <c r="G17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
@@ -1233,26 +1104,18 @@
       <c r="G18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -1260,16 +1123,8 @@
       <c r="G19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1283,26 +1138,18 @@
       <c r="G20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
@@ -1310,26 +1157,18 @@
       <c r="G21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -1337,26 +1176,18 @@
       <c r="G22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -1364,26 +1195,18 @@
       <c r="G23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -1391,26 +1214,18 @@
       <c r="G24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -1418,26 +1233,18 @@
       <c r="G25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -1445,26 +1252,18 @@
       <c r="G26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
@@ -1472,26 +1271,18 @@
       <c r="G27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
@@ -1499,87 +1290,24 @@
       <c r="G28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="F29" s="4">
         <v>2</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="4">
-        <v>2</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30">
-        <f t="shared" ref="I30" si="2">LEN(C30)</f>
-        <v>14</v>
-      </c>
-      <c r="J30">
-        <f t="shared" ref="J30" si="3">LEN(E30)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>